<commit_message>
Integrated the Excel data fetch utility with our framework Changes in file HomePageData.py and test_HomePage.py
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shubhangvats\PycharmProjects\pythonSelFramework\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F2EE898-07C1-4BE0-9F20-F93328C6A139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12292222-1571-4E72-A973-B4757E1746A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,9 +33,6 @@
     <t>first_name</t>
   </si>
   <si>
-    <t>last_name</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
@@ -109,6 +106,9 @@
   </si>
   <si>
     <t>Hgy1</t>
+  </si>
+  <si>
+    <t>password</t>
   </si>
 </sst>
 </file>
@@ -446,7 +446,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -457,16 +457,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -474,83 +474,83 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>